<commit_message>
Spilletd TC052 in to two parts and updated Excel
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="622"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="622" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Modules" sheetId="32" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="FilePath" sheetId="35" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TestCases!$A$1:$D$113</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TestCases!$A$1:$D$114</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Modules!$A$1:$R$27</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -37,7 +37,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C6" authorId="0">
+    <comment ref="C6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="333">
   <si>
     <t>Scenarios</t>
   </si>
@@ -892,9 +892,6 @@
     <t>PESmokeTc053_VerifySentEmailAndActivityFromCapitalCallPage</t>
   </si>
   <si>
-    <t>PESmokeTc052_VerifySentEmailAndActivityFromDrawdownPage</t>
-  </si>
-  <si>
     <t>PESmokeTc054_VerifyMailReceivedAndActivity</t>
   </si>
   <si>
@@ -1070,13 +1067,20 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>PESmokeTc052_1_VerifySentEmailAndActivityFromDrawdownPage</t>
+  </si>
+  <si>
+    <t>PESmokeTc052_2_VerifySentEmailAndActivityFromDrawdownPage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1341,7 +1345,133 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="110">
+  <dxfs count="122">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2790,31 +2920,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="H1:I17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="7" width="9.140625" style="1" collapsed="1"/>
-    <col min="8" max="8" width="15.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="15.7109375" collapsed="true"/>
+    <col min="2" max="7" style="1" width="9.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="8.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="11" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="8:9" s="15" customFormat="1" ht="16.5" thickBot="1">
+    <row r="1" spans="8:9" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H1" s="20" t="s">
         <v>72</v>
       </c>
@@ -2822,7 +2952,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="8:9" ht="15.75" thickBot="1">
+    <row r="2" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H2" s="19" t="s">
         <v>180</v>
       </c>
@@ -2830,74 +2960,74 @@
         <v>189</v>
       </c>
     </row>
-    <row r="3" spans="8:9" ht="15.75" thickBot="1">
+    <row r="3" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H3" s="19"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="8:9" ht="15.75" thickBot="1">
+    <row r="4" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H4" s="19"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="8:9" ht="15.75" thickBot="1">
+    <row r="5" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H5" s="19"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="8:9" ht="15.75" thickBot="1">
+    <row r="6" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H6" s="19"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="8:9" ht="15.75" thickBot="1">
+    <row r="7" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H7" s="19"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="8:9" ht="15.75" thickBot="1">
+    <row r="8" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H8" s="19"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="8:9" ht="15.75" thickBot="1">
+    <row r="9" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H9" s="19"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="8:9" ht="15.75" thickBot="1">
+    <row r="10" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H10" s="19"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="8:9" ht="15.75" thickBot="1">
+    <row r="11" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H11" s="19"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="8:9" ht="15.75" thickBot="1">
+    <row r="12" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H12" s="19"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="8:9" ht="15.75" thickBot="1">
+    <row r="13" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H13" s="19"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="8:9" ht="15.75" thickBot="1">
+    <row r="14" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H14" s="19"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="8:9" ht="15.75" thickBot="1">
+    <row r="15" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H15" s="19"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="8:9" ht="15.75" thickBot="1">
+    <row r="16" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H16" s="19"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="8:9" ht="15.75" thickBot="1">
+    <row r="17" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H17" s="19"/>
       <c r="I17" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I17">
-    <cfRule type="cellIs" dxfId="109" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I17">
-    <cfRule type="cellIs" dxfId="108" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2912,7 +3042,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2920,14 +3050,14 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="10" customFormat="1">
+    <row r="1" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
@@ -2944,7 +3074,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2952,15 +3082,15 @@
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="10" customFormat="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
@@ -2980,7 +3110,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -2988,14 +3118,14 @@
       <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="19" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="19" collapsed="1"/>
-    <col min="5" max="5" width="37.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="19" collapsed="1"/>
+    <col min="1" max="4" width="19.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="6" max="16384" width="19.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
@@ -3024,7 +3154,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -3045,7 +3175,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -3089,28 +3219,28 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="29.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="29.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="9" customFormat="1">
+    <row r="1" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>5</v>
       </c>
@@ -3130,7 +3260,7 @@
       </c>
       <c r="J1" s="12"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -3162,7 +3292,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>57</v>
       </c>
@@ -3182,7 +3312,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -3199,7 +3329,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>4</v>
       </c>
@@ -3207,72 +3337,72 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="4:4">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="4:4">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="4:4">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>24</v>
       </c>
@@ -3288,20 +3418,20 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="255.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="43.42578125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="255.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>246</v>
       </c>
@@ -3369,7 +3499,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>268</v>
       </c>
@@ -3377,17 +3507,17 @@
         <v>269</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="O4" s="22" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -3396,24 +3526,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E113"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E114"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C106" sqref="C106:C113"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="78" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="46.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.140625" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="78.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="46.5703125" collapsed="true"/>
+    <col min="5" max="16384" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="18" customFormat="1" ht="18" thickBot="1">
+    <row r="1" spans="1:5" s="18" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>32</v>
       </c>
@@ -3427,15 +3557,15 @@
         <v>2</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>186</v>
@@ -3444,67 +3574,67 @@
         <v>190</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>182</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D3" t="s">
-        <v>190</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A4" s="13" t="s">
+      <c r="C4" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
         <v>285</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D4" t="s">
-        <v>190</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A5" s="13" t="s">
+      <c r="C5" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
         <v>286</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D5" t="s">
-        <v>190</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A6" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>298</v>
-      </c>
       <c r="C6" s="3" t="s">
         <v>186</v>
       </c>
@@ -3512,10 +3642,10 @@
         <v>190</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>183</v>
       </c>
@@ -3529,10 +3659,10 @@
         <v>190</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>184</v>
       </c>
@@ -3546,10 +3676,10 @@
         <v>190</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>188</v>
       </c>
@@ -3563,12 +3693,12 @@
         <v>190</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B10" s="3">
         <v>5</v>
@@ -3580,12 +3710,12 @@
         <v>190</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B11" s="3">
         <v>5</v>
@@ -3597,10 +3727,10 @@
         <v>190</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>202</v>
       </c>
@@ -3614,10 +3744,10 @@
         <v>190</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>203</v>
       </c>
@@ -3631,10 +3761,10 @@
         <v>190</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>204</v>
       </c>
@@ -3648,12 +3778,12 @@
         <v>190</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B15" s="3">
         <v>9</v>
@@ -3665,12 +3795,12 @@
         <v>190</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B16" s="3">
         <v>9</v>
@@ -3682,10 +3812,10 @@
         <v>190</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>210</v>
       </c>
@@ -3699,12 +3829,12 @@
         <v>190</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B18" s="3">
         <v>11</v>
@@ -3716,12 +3846,12 @@
         <v>190</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B19" s="3">
         <v>12</v>
@@ -3733,12 +3863,12 @@
         <v>190</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
@@ -3748,12 +3878,12 @@
         <v>190</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B21" s="3">
         <v>13</v>
@@ -3765,12 +3895,12 @@
         <v>190</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B22" s="3">
         <v>14</v>
@@ -3782,12 +3912,12 @@
         <v>190</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B23" s="3">
         <v>15</v>
@@ -3799,12 +3929,12 @@
         <v>190</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B24" s="3">
         <v>16</v>
@@ -3816,12 +3946,12 @@
         <v>190</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
@@ -3831,12 +3961,12 @@
         <v>190</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
@@ -3846,12 +3976,12 @@
         <v>190</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B27" s="3">
         <v>17</v>
@@ -3863,10 +3993,10 @@
         <v>190</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
         <v>218</v>
       </c>
@@ -3880,10 +4010,10 @@
         <v>190</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
         <v>219</v>
       </c>
@@ -3897,12 +4027,12 @@
         <v>190</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B30" s="3">
         <v>20</v>
@@ -3914,12 +4044,12 @@
         <v>190</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3" t="s">
@@ -3929,10 +4059,10 @@
         <v>190</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
         <v>225</v>
       </c>
@@ -3946,12 +4076,12 @@
         <v>190</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B33" s="3">
         <v>22</v>
@@ -3963,10 +4093,10 @@
         <v>190</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" thickBot="1">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
         <v>226</v>
       </c>
@@ -3980,12 +4110,12 @@
         <v>190</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B35" s="3">
         <v>24</v>
@@ -3997,12 +4127,12 @@
         <v>190</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" thickBot="1">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B36" s="3">
         <v>25</v>
@@ -4014,12 +4144,12 @@
         <v>190</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B37" s="3">
         <v>25</v>
@@ -4031,12 +4161,12 @@
         <v>190</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B38" s="3">
         <v>26</v>
@@ -4048,12 +4178,12 @@
         <v>190</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B39" s="3">
         <v>27</v>
@@ -4065,12 +4195,12 @@
         <v>190</v>
       </c>
       <c r="E39" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B40" s="3">
         <v>28</v>
@@ -4082,10 +4212,10 @@
         <v>190</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
         <v>227</v>
       </c>
@@ -4099,10 +4229,10 @@
         <v>190</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="18" customHeight="1" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
         <v>231</v>
       </c>
@@ -4116,10 +4246,10 @@
         <v>190</v>
       </c>
       <c r="E42" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
         <v>185</v>
       </c>
@@ -4133,10 +4263,10 @@
         <v>190</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
         <v>187</v>
       </c>
@@ -4150,10 +4280,10 @@
         <v>190</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>191</v>
       </c>
@@ -4167,10 +4297,10 @@
         <v>190</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="15.75" thickBot="1">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
         <v>192</v>
       </c>
@@ -4184,10 +4314,10 @@
         <v>190</v>
       </c>
       <c r="E46" s="23" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="15.75" thickBot="1">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
         <v>193</v>
       </c>
@@ -4201,10 +4331,10 @@
         <v>190</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
         <v>194</v>
       </c>
@@ -4218,10 +4348,10 @@
         <v>190</v>
       </c>
       <c r="E48" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
         <v>195</v>
       </c>
@@ -4235,10 +4365,10 @@
         <v>190</v>
       </c>
       <c r="E49" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
         <v>235</v>
       </c>
@@ -4252,10 +4382,10 @@
         <v>190</v>
       </c>
       <c r="E50" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
         <v>236</v>
       </c>
@@ -4269,10 +4399,10 @@
         <v>190</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="13" t="s">
         <v>237</v>
       </c>
@@ -4286,10 +4416,10 @@
         <v>190</v>
       </c>
       <c r="E52" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="13" t="s">
         <v>240</v>
       </c>
@@ -4303,10 +4433,10 @@
         <v>190</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="13" t="s">
         <v>241</v>
       </c>
@@ -4320,10 +4450,10 @@
         <v>190</v>
       </c>
       <c r="E54" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="13" t="s">
         <v>242</v>
       </c>
@@ -4337,10 +4467,10 @@
         <v>190</v>
       </c>
       <c r="E55" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="13" t="s">
         <v>243</v>
       </c>
@@ -4354,12 +4484,12 @@
         <v>190</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="13" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B57" s="3">
         <v>44</v>
@@ -4371,12 +4501,12 @@
         <v>190</v>
       </c>
       <c r="E57" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="13" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B58" s="3">
         <v>44</v>
@@ -4388,12 +4518,12 @@
         <v>190</v>
       </c>
       <c r="E58" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="13" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B59" s="3">
         <v>44</v>
@@ -4405,12 +4535,12 @@
         <v>190</v>
       </c>
       <c r="E59" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="13" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B60" s="3">
         <v>45</v>
@@ -4422,12 +4552,12 @@
         <v>190</v>
       </c>
       <c r="E60" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="13" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B61" s="3">
         <v>45</v>
@@ -4439,10 +4569,10 @@
         <v>190</v>
       </c>
       <c r="E61" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
         <v>233</v>
       </c>
@@ -4456,10 +4586,10 @@
         <v>190</v>
       </c>
       <c r="E62" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
         <v>234</v>
       </c>
@@ -4473,10 +4603,10 @@
         <v>190</v>
       </c>
       <c r="E63" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
         <v>244</v>
       </c>
@@ -4490,10 +4620,10 @@
         <v>190</v>
       </c>
       <c r="E64" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
         <v>245</v>
       </c>
@@ -4507,12 +4637,12 @@
         <v>190</v>
       </c>
       <c r="E65" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="13" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B66" s="3">
         <v>50</v>
@@ -4524,12 +4654,12 @@
         <v>190</v>
       </c>
       <c r="E66" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B67" s="3">
         <v>50</v>
@@ -4541,10 +4671,10 @@
         <v>190</v>
       </c>
       <c r="E67" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="13" t="s">
         <v>268</v>
       </c>
@@ -4558,12 +4688,12 @@
         <v>190</v>
       </c>
       <c r="E68" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="13" t="s">
-        <v>272</v>
+        <v>331</v>
       </c>
       <c r="B69" s="3">
         <v>52</v>
@@ -4575,12 +4705,12 @@
         <v>190</v>
       </c>
       <c r="E69" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="13" t="s">
-        <v>318</v>
+        <v>332</v>
       </c>
       <c r="B70" s="3">
         <v>52</v>
@@ -4592,129 +4722,129 @@
         <v>190</v>
       </c>
       <c r="E70" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="B71" s="3">
+        <v>52</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D71" t="s">
+        <v>190</v>
+      </c>
+      <c r="E71" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="B72" s="3">
+        <v>53</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D72" t="s">
+        <v>190</v>
+      </c>
+      <c r="E72" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="B73" s="3">
+        <v>54</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D73" t="s">
+        <v>190</v>
+      </c>
+      <c r="E73" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="13" t="s">
         <v>319</v>
       </c>
-      <c r="B71" s="3">
-        <v>53</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D71" t="s">
-        <v>190</v>
-      </c>
-      <c r="E71" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A72" s="13" t="s">
+      <c r="B74" s="3">
+        <v>55</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D74" t="s">
+        <v>190</v>
+      </c>
+      <c r="E74" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D75" t="s">
+        <v>190</v>
+      </c>
+      <c r="E75" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="B72" s="3">
-        <v>54</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D72" t="s">
-        <v>190</v>
-      </c>
-      <c r="E72" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A73" s="13" t="s">
-        <v>320</v>
-      </c>
-      <c r="B73" s="3">
-        <v>55</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D73" t="s">
-        <v>190</v>
-      </c>
-      <c r="E73" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A74" s="13" t="s">
+      <c r="B76" s="3">
+        <v>56</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D76" t="s">
+        <v>190</v>
+      </c>
+      <c r="E76" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="B77" s="3">
+        <v>57</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D77" t="s">
+        <v>190</v>
+      </c>
+      <c r="E77" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="13" t="s">
         <v>321</v>
-      </c>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D74" t="s">
-        <v>190</v>
-      </c>
-      <c r="E74" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A75" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="B75" s="3">
-        <v>56</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D75" t="s">
-        <v>190</v>
-      </c>
-      <c r="E75" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A76" s="13" t="s">
-        <v>275</v>
-      </c>
-      <c r="B76" s="3">
-        <v>57</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D76" t="s">
-        <v>190</v>
-      </c>
-      <c r="E76" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A77" s="13" t="s">
-        <v>322</v>
-      </c>
-      <c r="B77" s="3">
-        <v>58</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D77" t="s">
-        <v>190</v>
-      </c>
-      <c r="E77" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A78" s="13" t="s">
-        <v>323</v>
       </c>
       <c r="B78" s="3">
         <v>58</v>
@@ -4726,33 +4856,33 @@
         <v>190</v>
       </c>
       <c r="E78" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="13" t="s">
-        <v>288</v>
+        <v>322</v>
       </c>
       <c r="B79" s="3">
+        <v>58</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D79" t="s">
+        <v>190</v>
+      </c>
+      <c r="E79" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="B80" s="3">
         <v>59</v>
       </c>
-      <c r="C79" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D79" t="s">
-        <v>190</v>
-      </c>
-      <c r="E79" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A80" s="13" t="s">
-        <v>324</v>
-      </c>
-      <c r="B80" s="3">
-        <v>60</v>
-      </c>
       <c r="C80" s="3" t="s">
         <v>186</v>
       </c>
@@ -4760,12 +4890,12 @@
         <v>190</v>
       </c>
       <c r="E80" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B81" s="3">
         <v>60</v>
@@ -4777,505 +4907,505 @@
         <v>190</v>
       </c>
       <c r="E81" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="13" t="s">
-        <v>289</v>
+        <v>324</v>
       </c>
       <c r="B82" s="3">
+        <v>60</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D82" t="s">
+        <v>190</v>
+      </c>
+      <c r="E82" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="B83" s="3">
         <v>61</v>
       </c>
-      <c r="C82" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D82" t="s">
-        <v>190</v>
-      </c>
-      <c r="E82" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A83" s="13" t="s">
+      <c r="C83" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D83" t="s">
+        <v>190</v>
+      </c>
+      <c r="E83" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="B83" s="3">
+      <c r="B84" s="3">
         <v>62</v>
       </c>
-      <c r="C83" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D83" t="s">
-        <v>190</v>
-      </c>
-      <c r="E83" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A84" s="13" t="s">
+      <c r="C84" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D84" t="s">
+        <v>190</v>
+      </c>
+      <c r="E84" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="B84" s="3">
+      <c r="B85" s="3">
         <v>63</v>
       </c>
-      <c r="C84" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D84" t="s">
-        <v>190</v>
-      </c>
-      <c r="E84" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A85" s="13" t="s">
+      <c r="C85" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D85" t="s">
+        <v>190</v>
+      </c>
+      <c r="E85" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="B85" s="3">
+      <c r="B86" s="3">
         <v>64</v>
       </c>
-      <c r="C85" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D85" t="s">
-        <v>190</v>
-      </c>
-      <c r="E85" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A86" s="13" t="s">
+      <c r="C86" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D86" t="s">
+        <v>190</v>
+      </c>
+      <c r="E86" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="B86" s="3">
+      <c r="B87" s="3">
         <v>65</v>
       </c>
-      <c r="C86" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D86" t="s">
-        <v>190</v>
-      </c>
-      <c r="E86" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A87" s="13" t="s">
+      <c r="C87" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D87" t="s">
+        <v>190</v>
+      </c>
+      <c r="E87" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="B87" s="3">
+      <c r="B88" s="3">
         <v>66</v>
       </c>
-      <c r="C87" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D87" t="s">
-        <v>190</v>
-      </c>
-      <c r="E87" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A88" s="13" t="s">
+      <c r="C88" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D88" t="s">
+        <v>190</v>
+      </c>
+      <c r="E88" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="B88" s="3">
+      <c r="B89" s="3">
         <v>67</v>
       </c>
-      <c r="C88" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D88" t="s">
-        <v>190</v>
-      </c>
-      <c r="E88" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A89" s="13" t="s">
+      <c r="C89" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D89" t="s">
+        <v>190</v>
+      </c>
+      <c r="E89" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="B89" s="3">
+      <c r="B90" s="3">
         <v>68</v>
       </c>
-      <c r="C89" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D89" t="s">
-        <v>190</v>
-      </c>
-      <c r="E89" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A90" s="13" t="s">
+      <c r="C90" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D90" t="s">
+        <v>190</v>
+      </c>
+      <c r="E90" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="B90" s="3">
+      <c r="B91" s="3">
         <v>69</v>
       </c>
-      <c r="C90" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D90" t="s">
-        <v>190</v>
-      </c>
-      <c r="E90" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A91" s="13" t="s">
+      <c r="C91" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D91" t="s">
+        <v>190</v>
+      </c>
+      <c r="E91" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="B91" s="3">
+      <c r="B92" s="3">
         <v>70</v>
       </c>
-      <c r="C91" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D91" t="s">
-        <v>190</v>
-      </c>
-      <c r="E91" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A92" s="13" t="s">
+      <c r="C92" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D92" t="s">
+        <v>190</v>
+      </c>
+      <c r="E92" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="B92" s="3">
+      <c r="B93" s="3">
         <v>71</v>
       </c>
-      <c r="C92" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D92" t="s">
-        <v>190</v>
-      </c>
-      <c r="E92" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A93" s="13" t="s">
+      <c r="C93" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D93" t="s">
+        <v>190</v>
+      </c>
+      <c r="E93" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="B93" s="3">
+      <c r="B94" s="3">
         <v>72</v>
       </c>
-      <c r="C93" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D93" t="s">
-        <v>190</v>
-      </c>
-      <c r="E93" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A94" s="13" t="s">
+      <c r="C94" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D94" t="s">
+        <v>190</v>
+      </c>
+      <c r="E94" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="B94" s="3">
+      <c r="B95" s="3">
         <v>73</v>
       </c>
-      <c r="C94" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D94" t="s">
-        <v>190</v>
-      </c>
-      <c r="E94" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A95" s="13" t="s">
+      <c r="C95" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D95" t="s">
+        <v>190</v>
+      </c>
+      <c r="E95" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="B95" s="3">
+      <c r="B96" s="3">
         <v>74</v>
       </c>
-      <c r="C95" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D95" t="s">
-        <v>190</v>
-      </c>
-      <c r="E95" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A96" s="13" t="s">
+      <c r="C96" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D96" t="s">
+        <v>190</v>
+      </c>
+      <c r="E96" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="B96" s="3">
+      <c r="B97" s="3">
         <v>75</v>
       </c>
-      <c r="C96" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D96" t="s">
-        <v>190</v>
-      </c>
-      <c r="E96" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A97" s="13" t="s">
+      <c r="C97" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D97" t="s">
+        <v>190</v>
+      </c>
+      <c r="E97" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="B97" s="3">
+      <c r="B98" s="3">
         <v>76</v>
       </c>
-      <c r="C97" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D97" t="s">
-        <v>190</v>
-      </c>
-      <c r="E97" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A98" s="13" t="s">
+      <c r="C98" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D98" t="s">
+        <v>190</v>
+      </c>
+      <c r="E98" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="B98" s="3">
+      <c r="B99" s="3">
         <v>77</v>
       </c>
-      <c r="C98" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D98" t="s">
-        <v>190</v>
-      </c>
-      <c r="E98" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A99" s="13" t="s">
+      <c r="C99" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D99" t="s">
+        <v>190</v>
+      </c>
+      <c r="E99" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="B99" s="3">
+      <c r="B100" s="3">
         <v>78</v>
       </c>
-      <c r="C99" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D99" t="s">
-        <v>190</v>
-      </c>
-      <c r="E99" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A100" s="13" t="s">
+      <c r="C100" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D100" t="s">
+        <v>190</v>
+      </c>
+      <c r="E100" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="B100" s="3">
+      <c r="B101" s="3">
         <v>79</v>
       </c>
-      <c r="C100" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D100" t="s">
-        <v>190</v>
-      </c>
-      <c r="E100" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A101" s="13" t="s">
+      <c r="C101" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D101" t="s">
+        <v>190</v>
+      </c>
+      <c r="E101" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="B101" s="3">
+      <c r="B102" s="3">
         <v>80</v>
       </c>
-      <c r="C101" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D101" t="s">
-        <v>190</v>
-      </c>
-      <c r="E101" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A102" s="13" t="s">
+      <c r="C102" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D102" t="s">
+        <v>190</v>
+      </c>
+      <c r="E102" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="B102" s="3">
+      <c r="B103" s="3">
         <v>81</v>
       </c>
-      <c r="C102" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D102" t="s">
-        <v>190</v>
-      </c>
-      <c r="E102" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A103" s="13" t="s">
+      <c r="C103" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D103" t="s">
+        <v>190</v>
+      </c>
+      <c r="E103" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="B103" s="3">
+      <c r="B104" s="3">
         <v>82</v>
       </c>
-      <c r="C103" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D103" t="s">
-        <v>190</v>
-      </c>
-      <c r="E103" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A104" s="13" t="s">
+      <c r="C104" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D104" t="s">
+        <v>190</v>
+      </c>
+      <c r="E104" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="B104" s="3">
+      <c r="B105" s="3">
         <v>83</v>
       </c>
-      <c r="C104" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D104" t="s">
-        <v>190</v>
-      </c>
-      <c r="E104" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A105" s="13" t="s">
+      <c r="C105" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D105" t="s">
+        <v>190</v>
+      </c>
+      <c r="E105" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="B105" s="3">
+      <c r="B106" s="3">
         <v>84</v>
       </c>
-      <c r="C105" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D105" t="s">
-        <v>190</v>
-      </c>
-      <c r="E105" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A106" s="13" t="s">
+      <c r="C106" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D106" t="s">
+        <v>190</v>
+      </c>
+      <c r="E106" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="B106" s="3">
+      <c r="B107" s="3">
         <v>85</v>
       </c>
-      <c r="C106" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D106" t="s">
-        <v>190</v>
-      </c>
-      <c r="E106" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A107" s="13" t="s">
+      <c r="C107" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D107" t="s">
+        <v>190</v>
+      </c>
+      <c r="E107" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="B107" s="3">
+      <c r="B108" s="3">
         <v>86</v>
       </c>
-      <c r="C107" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D107" t="s">
-        <v>331</v>
-      </c>
-      <c r="E107" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A108" s="13" t="s">
+      <c r="C108" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D108" t="s">
+        <v>190</v>
+      </c>
+      <c r="E108" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="B108" s="3">
+      <c r="B109" s="3">
         <v>87</v>
       </c>
-      <c r="C108" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D108" t="s">
-        <v>331</v>
-      </c>
-      <c r="E108" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A109" s="13" t="s">
+      <c r="C109" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D109" t="s">
+        <v>190</v>
+      </c>
+      <c r="E109" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="B109" s="3">
+      <c r="B110" s="3">
         <v>88</v>
       </c>
-      <c r="C109" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D109" t="s">
-        <v>331</v>
-      </c>
-      <c r="E109" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A110" s="13" t="s">
-        <v>326</v>
-      </c>
-      <c r="B110" s="3">
-        <v>89</v>
-      </c>
       <c r="C110" s="3" t="s">
         <v>186</v>
       </c>
       <c r="D110" t="s">
-        <v>331</v>
+        <v>190</v>
       </c>
       <c r="E110" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="13" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B111" s="3">
         <v>89</v>
@@ -5284,449 +5414,488 @@
         <v>186</v>
       </c>
       <c r="D111" t="s">
-        <v>331</v>
+        <v>190</v>
       </c>
       <c r="E111" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" ht="15.75" thickBot="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="B112" s="3">
+        <v>89</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D112" t="s">
+        <v>190</v>
+      </c>
+      <c r="E112" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="B112" s="3">
+      <c r="B113" s="3">
         <v>90</v>
       </c>
-      <c r="C112" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D112" t="s">
-        <v>331</v>
-      </c>
-      <c r="E112" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A113" s="13" t="s">
+      <c r="C113" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D113" t="s">
+        <v>190</v>
+      </c>
+      <c r="E113" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="B113" s="3">
+      <c r="B114" s="3">
         <v>91</v>
       </c>
-      <c r="C113" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D113" t="s">
-        <v>331</v>
-      </c>
-      <c r="E113" s="23" t="s">
-        <v>293</v>
+      <c r="C114" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D114" t="s">
+        <v>190</v>
+      </c>
+      <c r="E114" s="23" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D3:D9 D12:D15 D17:D23 D38:D57 D27:D35 D62:D66 D68:D69 D71:D76 D78:D80 D82:D89">
-    <cfRule type="containsText" dxfId="107" priority="184" operator="containsText" text="Skip:">
+  <conditionalFormatting sqref="D3:D9 D12:D15 D17:D23 D38:D57 D27:D35 D62:D66 D68:D69 D72:D77 D79:D81 D83:D90">
+    <cfRule type="containsText" dxfId="119" priority="190" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="185" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="118" priority="191" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="186" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="117" priority="192" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D90:D92">
-    <cfRule type="containsText" dxfId="104" priority="139" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D90)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="140" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D90)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="141" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D90)))</formula>
+  <conditionalFormatting sqref="D91:D93">
+    <cfRule type="containsText" dxfId="116" priority="145" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D91)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="115" priority="146" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D91)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="114" priority="147" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D91)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D90:D92">
-    <cfRule type="containsText" dxfId="101" priority="136" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D90)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="137" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D90)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="138" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D90)))</formula>
+  <conditionalFormatting sqref="D91:D93">
+    <cfRule type="containsText" dxfId="113" priority="142" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D91)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="112" priority="143" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D91)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="111" priority="144" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D91)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="98" priority="106" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="110" priority="112" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="107" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="109" priority="113" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="108" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="108" priority="114" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="95" priority="103" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="107" priority="109" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="104" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="106" priority="110" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="105" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="105" priority="111" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E9 E12:E15 E27:E35 E38:E57 E62:E66 E68:E69 E71:E76 E78:E80 E82:E113 E17:E23">
-    <cfRule type="cellIs" dxfId="92" priority="100" operator="equal">
+  <conditionalFormatting sqref="E2:E9 E12:E15 E27:E35 E38:E57 E62:E66 E68:E69 E72:E77 E79:E81 E83:E114 E17:E23">
+    <cfRule type="cellIs" dxfId="104" priority="106" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="107" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="108" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="containsText" dxfId="89" priority="97" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="101" priority="103" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="98" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="100" priority="104" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="99" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="99" priority="105" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="86" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="100" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="101" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="102" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="containsText" dxfId="83" priority="91" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="95" priority="97" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="92" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="94" priority="98" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="93" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="93" priority="99" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="80" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="94" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="95" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="96" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="containsText" dxfId="77" priority="85" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="89" priority="91" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="86" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="88" priority="92" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="87" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="87" priority="93" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="74" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="88" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="89" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="90" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24:D26">
-    <cfRule type="containsText" dxfId="71" priority="79" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="83" priority="85" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="80" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="82" priority="86" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="81" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="81" priority="87" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24:E26">
-    <cfRule type="cellIs" dxfId="68" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="82" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="83" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="84" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="cellIs" dxfId="65" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="70" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="71" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="72" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="containsText" dxfId="62" priority="73" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="74" priority="79" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="74" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="73" priority="80" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="75" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="72" priority="81" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="cellIs" dxfId="59" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="76" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="77" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="78" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37">
-    <cfRule type="containsText" dxfId="56" priority="67" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="68" priority="73" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="68" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="67" priority="74" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="69" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="66" priority="75" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E61">
-    <cfRule type="cellIs" dxfId="53" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="58" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="59" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="60" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D60">
-    <cfRule type="containsText" dxfId="50" priority="61" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="62" priority="67" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D60)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="62" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="61" priority="68" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D60)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="63" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="60" priority="69" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E60">
-    <cfRule type="cellIs" dxfId="47" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="64" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="65" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="66" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D61">
-    <cfRule type="containsText" dxfId="44" priority="55" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="56" priority="61" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D61)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="56" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="55" priority="62" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D61)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="57" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="54" priority="63" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67">
-    <cfRule type="containsText" dxfId="41" priority="49" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="53" priority="55" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="50" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="52" priority="56" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="51" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="51" priority="57" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D67)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67">
-    <cfRule type="cellIs" dxfId="38" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="52" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="53" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="54" operator="equal">
       <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D71">
+    <cfRule type="containsText" dxfId="47" priority="49" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D71)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="50" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D71)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="45" priority="51" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D71)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E71">
+    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="47" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="48" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D78">
+    <cfRule type="containsText" dxfId="41" priority="43" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D78)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="44" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D78)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="39" priority="45" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D78)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E78">
+    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="41" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="42" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D82">
+    <cfRule type="containsText" dxfId="35" priority="37" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D82)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="38" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D82)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="39" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D82)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E82">
+    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="35" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="36" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D58">
+    <cfRule type="containsText" dxfId="29" priority="22" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="23" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="24" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58">
+    <cfRule type="cellIs" dxfId="26" priority="19" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="20" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="21" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D59">
+    <cfRule type="containsText" dxfId="23" priority="16" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D59)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="17" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D59)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="18" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E59">
+    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="14" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="15" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D94:D114">
+    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D94)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="11" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D94)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D94)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D94:D114">
+    <cfRule type="containsText" dxfId="14" priority="7" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D94)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D94)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D94)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="containsText" dxfId="35" priority="43" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D70)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="44" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D70)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="45" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D70)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E70">
-    <cfRule type="cellIs" dxfId="32" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D77">
-    <cfRule type="containsText" dxfId="29" priority="37" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D77)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="38" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D77)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="39" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D77)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E77">
-    <cfRule type="cellIs" dxfId="26" priority="34" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="35" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="36" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D81">
-    <cfRule type="containsText" dxfId="23" priority="31" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D81)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="32" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D81)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="33" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D81)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E81">
-    <cfRule type="cellIs" dxfId="20" priority="28" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="29" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="30" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D58">
-    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D58)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D58)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E58">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D59">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D59)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D59)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E59">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D93:D113">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D93)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D93)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D93)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D93:D113">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D93)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D93)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D93)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="C1"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C113">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C114">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E113">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E114">
       <formula1>"High,Low"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5736,7 +5905,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5744,30 +5913,30 @@
       <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="43.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.42578125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="20" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="43.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="43.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="17" customFormat="1">
+    <row r="1" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>33</v>
       </c>
@@ -5838,7 +6007,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -5849,7 +6018,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>84</v>
       </c>
@@ -5857,7 +6026,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>86</v>
       </c>
@@ -5865,7 +6034,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>88</v>
       </c>
@@ -5873,7 +6042,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>89</v>
       </c>
@@ -5902,7 +6071,7 @@
         <v>554477331</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>94</v>
       </c>
@@ -5910,7 +6079,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>95</v>
       </c>
@@ -5918,7 +6087,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>96</v>
       </c>
@@ -5947,7 +6116,7 @@
         <v>330548934</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>100</v>
       </c>
@@ -5955,7 +6124,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>101</v>
       </c>
@@ -5970,7 +6139,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5978,15 +6147,15 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="40.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="40.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="10" customFormat="1">
+    <row r="1" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
@@ -6006,25 +6175,25 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
@@ -6047,7 +6216,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>166</v>
       </c>
@@ -6070,7 +6239,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>166</v>
       </c>
@@ -6087,7 +6256,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>166</v>
       </c>
@@ -6104,7 +6273,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>175</v>
       </c>
@@ -6121,7 +6290,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>175</v>
       </c>
@@ -6138,7 +6307,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>177</v>
       </c>
@@ -6155,7 +6324,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>177</v>
       </c>
@@ -6172,7 +6341,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>177</v>
       </c>
@@ -6195,55 +6364,55 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AM7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AL7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="37.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="27.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="27.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="29.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="24" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.140625" collapsed="1"/>
-    <col min="28" max="28" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="15" style="16" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="30.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="29.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="22" max="24" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="27" max="27" width="9.140625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="35" max="35" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="37" max="37" customWidth="true" style="16" width="15.0" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="30.42578125" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="10" customFormat="1">
+    <row r="1" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
@@ -6294,7 +6463,7 @@
       </c>
       <c r="AL1" s="8"/>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>46</v>
       </c>
@@ -6308,7 +6477,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>46</v>
       </c>
@@ -6322,7 +6491,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>46</v>
       </c>
@@ -6336,7 +6505,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>46</v>
       </c>
@@ -6350,7 +6519,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>46</v>
       </c>
@@ -6364,7 +6533,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>123</v>
       </c>
@@ -6401,29 +6570,29 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="59.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="24.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="36" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="59.28515625" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="36.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
@@ -6446,7 +6615,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>139</v>
       </c>
@@ -6469,7 +6638,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>143</v>
       </c>
@@ -6492,7 +6661,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>146</v>
       </c>
@@ -6522,7 +6691,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6530,18 +6699,18 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
@@ -6570,20 +6739,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:B7"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="26.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>33</v>
       </c>
@@ -6591,7 +6760,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>149</v>
       </c>
@@ -6599,7 +6768,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>151</v>
       </c>
@@ -6607,7 +6776,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>153</v>
       </c>

</xml_diff>

<commit_message>
update scenario number test case file
Signed-off-by: Ankit Jaiswal <ajaiswal@navatargroup.com>
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA43E7E-D558-47A0-BD10-4475B355B733}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98EA471-C692-4F45-A969-6787BE617AD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="622" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2264,8 +2264,8 @@
   <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2452,7 +2452,7 @@
         <v>98</v>
       </c>
       <c r="B11" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>11</v>
@@ -2469,7 +2469,7 @@
         <v>27</v>
       </c>
       <c r="B12" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>11</v>
@@ -2486,7 +2486,7 @@
         <v>28</v>
       </c>
       <c r="B13" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>11</v>
@@ -2503,7 +2503,7 @@
         <v>29</v>
       </c>
       <c r="B14" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>11</v>
@@ -2520,7 +2520,7 @@
         <v>99</v>
       </c>
       <c r="B15" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>11</v>
@@ -2537,7 +2537,7 @@
         <v>100</v>
       </c>
       <c r="B16" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>11</v>
@@ -2554,7 +2554,7 @@
         <v>35</v>
       </c>
       <c r="B17" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>11</v>
@@ -2571,7 +2571,7 @@
         <v>75</v>
       </c>
       <c r="B18" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>11</v>
@@ -2588,7 +2588,7 @@
         <v>102</v>
       </c>
       <c r="B19" s="2">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>11</v>
@@ -2604,7 +2604,9 @@
       <c r="A20" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2">
+        <v>14</v>
+      </c>
       <c r="C20" s="2" t="s">
         <v>11</v>
       </c>
@@ -2620,7 +2622,7 @@
         <v>76</v>
       </c>
       <c r="B21" s="2">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>11</v>
@@ -2637,7 +2639,7 @@
         <v>77</v>
       </c>
       <c r="B22" s="2">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>11</v>
@@ -2654,7 +2656,7 @@
         <v>78</v>
       </c>
       <c r="B23" s="2">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>11</v>
@@ -2671,7 +2673,7 @@
         <v>103</v>
       </c>
       <c r="B24" s="2">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>11</v>
@@ -2687,7 +2689,9 @@
       <c r="A25" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B25" s="2"/>
+      <c r="B25" s="2">
+        <v>20</v>
+      </c>
       <c r="C25" s="2" t="s">
         <v>11</v>
       </c>
@@ -2702,7 +2706,9 @@
       <c r="A26" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B26" s="2"/>
+      <c r="B26" s="2">
+        <v>21</v>
+      </c>
       <c r="C26" s="2" t="s">
         <v>11</v>
       </c>
@@ -2718,7 +2724,7 @@
         <v>107</v>
       </c>
       <c r="B27" s="2">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>11</v>
@@ -2735,7 +2741,7 @@
         <v>43</v>
       </c>
       <c r="B28" s="2">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>11</v>
@@ -2752,7 +2758,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="2">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>11</v>
@@ -2769,7 +2775,7 @@
         <v>108</v>
       </c>
       <c r="B30" s="2">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>11</v>
@@ -2785,7 +2791,9 @@
       <c r="A31" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B31" s="2"/>
+      <c r="B31" s="2">
+        <v>26</v>
+      </c>
       <c r="C31" s="2" t="s">
         <v>11</v>
       </c>
@@ -2801,7 +2809,7 @@
         <v>50</v>
       </c>
       <c r="B32" s="2">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>11</v>
@@ -2818,7 +2826,7 @@
         <v>79</v>
       </c>
       <c r="B33" s="2">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>11</v>
@@ -2835,7 +2843,7 @@
         <v>51</v>
       </c>
       <c r="B34" s="2">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>11</v>
@@ -2852,7 +2860,7 @@
         <v>80</v>
       </c>
       <c r="B35" s="2">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>11</v>
@@ -2869,7 +2877,7 @@
         <v>110</v>
       </c>
       <c r="B36" s="2">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>11</v>
@@ -2886,7 +2894,7 @@
         <v>111</v>
       </c>
       <c r="B37" s="2">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>11</v>
@@ -2903,7 +2911,7 @@
         <v>81</v>
       </c>
       <c r="B38" s="2">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>11</v>
@@ -2920,7 +2928,7 @@
         <v>82</v>
       </c>
       <c r="B39" s="2">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>11</v>
@@ -2937,7 +2945,7 @@
         <v>83</v>
       </c>
       <c r="B40" s="2">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>11</v>
@@ -2954,7 +2962,7 @@
         <v>52</v>
       </c>
       <c r="B41" s="2">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>11</v>
@@ -2971,7 +2979,7 @@
         <v>56</v>
       </c>
       <c r="B42" s="2">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>11</v>
@@ -2988,7 +2996,7 @@
         <v>10</v>
       </c>
       <c r="B43" s="2">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>11</v>
@@ -3005,7 +3013,7 @@
         <v>12</v>
       </c>
       <c r="B44" s="2">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>11</v>
@@ -3022,7 +3030,7 @@
         <v>16</v>
       </c>
       <c r="B45" s="2">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>11</v>
@@ -3039,7 +3047,7 @@
         <v>17</v>
       </c>
       <c r="B46" s="2">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>11</v>
@@ -3056,7 +3064,7 @@
         <v>18</v>
       </c>
       <c r="B47" s="2">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>11</v>
@@ -3073,7 +3081,7 @@
         <v>19</v>
       </c>
       <c r="B48" s="2">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>11</v>
@@ -3090,7 +3098,7 @@
         <v>20</v>
       </c>
       <c r="B49" s="2">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>11</v>
@@ -3107,7 +3115,7 @@
         <v>60</v>
       </c>
       <c r="B50" s="2">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>11</v>
@@ -3124,7 +3132,7 @@
         <v>61</v>
       </c>
       <c r="B51" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>11</v>
@@ -3141,7 +3149,7 @@
         <v>62</v>
       </c>
       <c r="B52" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>11</v>
@@ -3158,7 +3166,7 @@
         <v>65</v>
       </c>
       <c r="B53" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>11</v>
@@ -3175,7 +3183,7 @@
         <v>66</v>
       </c>
       <c r="B54" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>11</v>
@@ -3192,7 +3200,7 @@
         <v>67</v>
       </c>
       <c r="B55" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>11</v>
@@ -3209,7 +3217,7 @@
         <v>68</v>
       </c>
       <c r="B56" s="2">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>11</v>
@@ -3226,7 +3234,7 @@
         <v>126</v>
       </c>
       <c r="B57" s="2">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>11</v>
@@ -3243,7 +3251,7 @@
         <v>127</v>
       </c>
       <c r="B58" s="2">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>11</v>
@@ -3260,7 +3268,7 @@
         <v>112</v>
       </c>
       <c r="B59" s="2">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>11</v>
@@ -3277,7 +3285,7 @@
         <v>113</v>
       </c>
       <c r="B60" s="2">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>11</v>
@@ -3294,7 +3302,7 @@
         <v>58</v>
       </c>
       <c r="B61" s="2">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>11</v>
@@ -3311,7 +3319,7 @@
         <v>59</v>
       </c>
       <c r="B62" s="2">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>11</v>
@@ -3328,7 +3336,7 @@
         <v>69</v>
       </c>
       <c r="B63" s="2">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>11</v>
@@ -3345,7 +3353,7 @@
         <v>70</v>
       </c>
       <c r="B64" s="2">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>11</v>
@@ -3362,7 +3370,7 @@
         <v>114</v>
       </c>
       <c r="B65" s="2">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>11</v>
@@ -3379,7 +3387,7 @@
         <v>115</v>
       </c>
       <c r="B66" s="2">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>11</v>
@@ -3396,7 +3404,7 @@
         <v>71</v>
       </c>
       <c r="B67" s="2">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>11</v>
@@ -3413,7 +3421,7 @@
         <v>128</v>
       </c>
       <c r="B68" s="2">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>11</v>
@@ -3430,7 +3438,7 @@
         <v>129</v>
       </c>
       <c r="B69" s="2">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>11</v>
@@ -3447,7 +3455,7 @@
         <v>116</v>
       </c>
       <c r="B70" s="2">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>11</v>
@@ -3464,7 +3472,7 @@
         <v>117</v>
       </c>
       <c r="B71" s="2">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>11</v>
@@ -3481,7 +3489,7 @@
         <v>72</v>
       </c>
       <c r="B72" s="2">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>11</v>
@@ -3498,7 +3506,7 @@
         <v>118</v>
       </c>
       <c r="B73" s="2">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>11</v>
@@ -3514,7 +3522,9 @@
       <c r="A74" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B74" s="2"/>
+      <c r="B74" s="2">
+        <v>64</v>
+      </c>
       <c r="C74" s="2" t="s">
         <v>11</v>
       </c>
@@ -3530,7 +3540,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="2">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>11</v>
@@ -3547,7 +3557,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="2">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>11</v>
@@ -3564,7 +3574,7 @@
         <v>120</v>
       </c>
       <c r="B77" s="2">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>11</v>
@@ -3581,7 +3591,7 @@
         <v>121</v>
       </c>
       <c r="B78" s="2">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>11</v>
@@ -3598,7 +3608,7 @@
         <v>87</v>
       </c>
       <c r="B79" s="2">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>11</v>
@@ -3615,7 +3625,7 @@
         <v>122</v>
       </c>
       <c r="B80" s="2">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>11</v>
@@ -3632,7 +3642,7 @@
         <v>123</v>
       </c>
       <c r="B81" s="2">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>11</v>
@@ -3649,7 +3659,7 @@
         <v>88</v>
       </c>
       <c r="B82" s="2">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>11</v>
@@ -3666,7 +3676,7 @@
         <v>21</v>
       </c>
       <c r="B83" s="2">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>11</v>
@@ -3683,7 +3693,7 @@
         <v>22</v>
       </c>
       <c r="B84" s="2">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>11</v>
@@ -3700,7 +3710,7 @@
         <v>23</v>
       </c>
       <c r="B85" s="2">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>11</v>
@@ -3717,7 +3727,7 @@
         <v>24</v>
       </c>
       <c r="B86" s="2">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>11</v>
@@ -3734,7 +3744,7 @@
         <v>25</v>
       </c>
       <c r="B87" s="2">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>11</v>
@@ -3751,7 +3761,7 @@
         <v>26</v>
       </c>
       <c r="B88" s="2">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>11</v>
@@ -3768,7 +3778,7 @@
         <v>30</v>
       </c>
       <c r="B89" s="2">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>11</v>
@@ -3785,7 +3795,7 @@
         <v>31</v>
       </c>
       <c r="B90" s="2">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>11</v>
@@ -3802,7 +3812,7 @@
         <v>32</v>
       </c>
       <c r="B91" s="2">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>11</v>
@@ -3819,7 +3829,7 @@
         <v>33</v>
       </c>
       <c r="B92" s="2">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>11</v>
@@ -3836,7 +3846,7 @@
         <v>34</v>
       </c>
       <c r="B93" s="2">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>11</v>
@@ -3853,7 +3863,7 @@
         <v>40</v>
       </c>
       <c r="B94" s="2">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>11</v>
@@ -3870,7 +3880,7 @@
         <v>36</v>
       </c>
       <c r="B95" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>11</v>
@@ -3887,7 +3897,7 @@
         <v>37</v>
       </c>
       <c r="B96" s="2">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>11</v>
@@ -3904,7 +3914,7 @@
         <v>38</v>
       </c>
       <c r="B97" s="2">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>11</v>
@@ -3921,7 +3931,7 @@
         <v>39</v>
       </c>
       <c r="B98" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>11</v>
@@ -3938,7 +3948,7 @@
         <v>41</v>
       </c>
       <c r="B99" s="2">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>11</v>
@@ -3955,7 +3965,7 @@
         <v>42</v>
       </c>
       <c r="B100" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>11</v>
@@ -3972,7 +3982,7 @@
         <v>45</v>
       </c>
       <c r="B101" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>11</v>
@@ -3989,7 +3999,7 @@
         <v>46</v>
       </c>
       <c r="B102" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>11</v>
@@ -4006,7 +4016,7 @@
         <v>47</v>
       </c>
       <c r="B103" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>11</v>
@@ -4023,7 +4033,7 @@
         <v>48</v>
       </c>
       <c r="B104" s="2">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>11</v>
@@ -4040,7 +4050,7 @@
         <v>49</v>
       </c>
       <c r="B105" s="2">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>11</v>
@@ -4057,7 +4067,7 @@
         <v>53</v>
       </c>
       <c r="B106" s="2">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>11</v>
@@ -4074,7 +4084,7 @@
         <v>54</v>
       </c>
       <c r="B107" s="2">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>11</v>
@@ -4091,7 +4101,7 @@
         <v>55</v>
       </c>
       <c r="B108" s="2">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>11</v>
@@ -4108,7 +4118,7 @@
         <v>57</v>
       </c>
       <c r="B109" s="2">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>11</v>
@@ -4125,7 +4135,7 @@
         <v>124</v>
       </c>
       <c r="B110" s="2">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>11</v>
@@ -4142,7 +4152,7 @@
         <v>125</v>
       </c>
       <c r="B111" s="2">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>11</v>
@@ -4159,7 +4169,7 @@
         <v>63</v>
       </c>
       <c r="B112" s="2">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>11</v>
@@ -4176,7 +4186,7 @@
         <v>64</v>
       </c>
       <c r="B113" s="2">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
update tc number in excel sheet
Signed-off-by: Ankit Jaiswal <ajaiswal@navatargroup.com>
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE92DB9-41C2-4F0D-B0A3-18BA586FF20D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="622" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="622" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Modules" sheetId="32" r:id="rId1"/>
@@ -15,7 +16,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TestCases!$A$1:$D$113</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Modules!$A$1:$R$27</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
@@ -494,7 +495,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2148,7 +2149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="H1:I17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
@@ -2253,7 +2254,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I2:I17">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I2:I17" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2263,12 +2264,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B116" sqref="B116"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B59" sqref="B59:B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2455,7 +2456,7 @@
         <v>123</v>
       </c>
       <c r="B11" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>11</v>
@@ -2472,7 +2473,7 @@
         <v>27</v>
       </c>
       <c r="B12" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>11</v>
@@ -2489,7 +2490,7 @@
         <v>28</v>
       </c>
       <c r="B13" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>11</v>
@@ -2506,7 +2507,7 @@
         <v>29</v>
       </c>
       <c r="B14" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>11</v>
@@ -2523,7 +2524,7 @@
         <v>124</v>
       </c>
       <c r="B15" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>11</v>
@@ -2540,7 +2541,7 @@
         <v>125</v>
       </c>
       <c r="B16" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>11</v>
@@ -2557,7 +2558,7 @@
         <v>35</v>
       </c>
       <c r="B17" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>11</v>
@@ -2574,7 +2575,7 @@
         <v>99</v>
       </c>
       <c r="B18" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>11</v>
@@ -2591,7 +2592,7 @@
         <v>127</v>
       </c>
       <c r="B19" s="2">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>11</v>
@@ -2607,7 +2608,9 @@
       <c r="A20" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2">
+        <v>14</v>
+      </c>
       <c r="C20" s="2" t="s">
         <v>11</v>
       </c>
@@ -2623,7 +2626,7 @@
         <v>100</v>
       </c>
       <c r="B21" s="2">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>11</v>
@@ -2640,7 +2643,7 @@
         <v>101</v>
       </c>
       <c r="B22" s="2">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>11</v>
@@ -2657,7 +2660,7 @@
         <v>102</v>
       </c>
       <c r="B23" s="2">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>11</v>
@@ -2674,7 +2677,7 @@
         <v>128</v>
       </c>
       <c r="B24" s="2">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>11</v>
@@ -2690,7 +2693,9 @@
       <c r="A25" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B25" s="2"/>
+      <c r="B25" s="2">
+        <v>20</v>
+      </c>
       <c r="C25" s="2" t="s">
         <v>11</v>
       </c>
@@ -2705,7 +2710,9 @@
       <c r="A26" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B26" s="2"/>
+      <c r="B26" s="2">
+        <v>21</v>
+      </c>
       <c r="C26" s="2" t="s">
         <v>11</v>
       </c>
@@ -2721,7 +2728,7 @@
         <v>132</v>
       </c>
       <c r="B27" s="2">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>11</v>
@@ -2738,7 +2745,7 @@
         <v>43</v>
       </c>
       <c r="B28" s="2">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>11</v>
@@ -2755,7 +2762,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="2">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>11</v>
@@ -2772,7 +2779,7 @@
         <v>133</v>
       </c>
       <c r="B30" s="2">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>11</v>
@@ -2788,7 +2795,9 @@
       <c r="A31" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="B31" s="2"/>
+      <c r="B31" s="2">
+        <v>26</v>
+      </c>
       <c r="C31" s="2" t="s">
         <v>11</v>
       </c>
@@ -2804,7 +2813,7 @@
         <v>50</v>
       </c>
       <c r="B32" s="2">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>11</v>
@@ -2821,7 +2830,7 @@
         <v>103</v>
       </c>
       <c r="B33" s="2">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>11</v>
@@ -2838,7 +2847,7 @@
         <v>51</v>
       </c>
       <c r="B34" s="2">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>11</v>
@@ -2855,7 +2864,7 @@
         <v>104</v>
       </c>
       <c r="B35" s="2">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>11</v>
@@ -2872,7 +2881,7 @@
         <v>135</v>
       </c>
       <c r="B36" s="2">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>11</v>
@@ -2889,7 +2898,7 @@
         <v>136</v>
       </c>
       <c r="B37" s="2">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>11</v>
@@ -2906,7 +2915,7 @@
         <v>105</v>
       </c>
       <c r="B38" s="2">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>11</v>
@@ -2923,7 +2932,7 @@
         <v>106</v>
       </c>
       <c r="B39" s="2">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>11</v>
@@ -2940,7 +2949,7 @@
         <v>107</v>
       </c>
       <c r="B40" s="2">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>11</v>
@@ -2957,7 +2966,7 @@
         <v>52</v>
       </c>
       <c r="B41" s="2">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>11</v>
@@ -2974,7 +2983,7 @@
         <v>56</v>
       </c>
       <c r="B42" s="2">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>11</v>
@@ -2991,7 +3000,7 @@
         <v>10</v>
       </c>
       <c r="B43" s="2">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>11</v>
@@ -3008,7 +3017,7 @@
         <v>12</v>
       </c>
       <c r="B44" s="2">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>11</v>
@@ -3025,7 +3034,7 @@
         <v>16</v>
       </c>
       <c r="B45" s="2">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>11</v>
@@ -3042,7 +3051,7 @@
         <v>17</v>
       </c>
       <c r="B46" s="2">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>11</v>
@@ -3059,7 +3068,7 @@
         <v>18</v>
       </c>
       <c r="B47" s="2">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>11</v>
@@ -3076,7 +3085,7 @@
         <v>19</v>
       </c>
       <c r="B48" s="2">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>11</v>
@@ -3093,7 +3102,7 @@
         <v>20</v>
       </c>
       <c r="B49" s="2">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>11</v>
@@ -3110,7 +3119,7 @@
         <v>60</v>
       </c>
       <c r="B50" s="2">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>11</v>
@@ -3127,7 +3136,7 @@
         <v>61</v>
       </c>
       <c r="B51" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>11</v>
@@ -3144,7 +3153,7 @@
         <v>62</v>
       </c>
       <c r="B52" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>11</v>
@@ -3161,7 +3170,7 @@
         <v>65</v>
       </c>
       <c r="B53" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>11</v>
@@ -3178,7 +3187,7 @@
         <v>66</v>
       </c>
       <c r="B54" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>11</v>
@@ -3195,7 +3204,7 @@
         <v>67</v>
       </c>
       <c r="B55" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>11</v>
@@ -3212,7 +3221,7 @@
         <v>68</v>
       </c>
       <c r="B56" s="2">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>11</v>
@@ -3229,7 +3238,7 @@
         <v>151</v>
       </c>
       <c r="B57" s="2">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>11</v>
@@ -3246,7 +3255,7 @@
         <v>152</v>
       </c>
       <c r="B58" s="2">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>11</v>
@@ -3263,7 +3272,7 @@
         <v>137</v>
       </c>
       <c r="B59" s="2">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>11</v>
@@ -3280,7 +3289,7 @@
         <v>138</v>
       </c>
       <c r="B60" s="2">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>11</v>
@@ -3297,7 +3306,7 @@
         <v>58</v>
       </c>
       <c r="B61" s="2">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>11</v>
@@ -3314,7 +3323,7 @@
         <v>59</v>
       </c>
       <c r="B62" s="2">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>11</v>
@@ -3331,7 +3340,7 @@
         <v>69</v>
       </c>
       <c r="B63" s="2">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>11</v>
@@ -3348,7 +3357,7 @@
         <v>70</v>
       </c>
       <c r="B64" s="2">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>11</v>
@@ -3365,7 +3374,7 @@
         <v>139</v>
       </c>
       <c r="B65" s="2">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>11</v>
@@ -3382,7 +3391,7 @@
         <v>140</v>
       </c>
       <c r="B66" s="2">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>11</v>
@@ -3399,7 +3408,7 @@
         <v>93</v>
       </c>
       <c r="B67" s="2">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>11</v>
@@ -3416,7 +3425,7 @@
         <v>153</v>
       </c>
       <c r="B68" s="2">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>11</v>
@@ -3433,7 +3442,7 @@
         <v>154</v>
       </c>
       <c r="B69" s="2">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>11</v>
@@ -3450,7 +3459,7 @@
         <v>141</v>
       </c>
       <c r="B70" s="2">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>11</v>
@@ -3467,7 +3476,7 @@
         <v>142</v>
       </c>
       <c r="B71" s="2">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>11</v>
@@ -3484,7 +3493,7 @@
         <v>96</v>
       </c>
       <c r="B72" s="2">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>11</v>
@@ -3501,7 +3510,7 @@
         <v>143</v>
       </c>
       <c r="B73" s="2">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>11</v>
@@ -3517,7 +3526,9 @@
       <c r="A74" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="B74" s="2"/>
+      <c r="B74" s="2">
+        <v>64</v>
+      </c>
       <c r="C74" s="2" t="s">
         <v>11</v>
       </c>
@@ -3533,7 +3544,7 @@
         <v>97</v>
       </c>
       <c r="B75" s="2">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>11</v>
@@ -3550,7 +3561,7 @@
         <v>98</v>
       </c>
       <c r="B76" s="2">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>11</v>
@@ -3567,7 +3578,7 @@
         <v>145</v>
       </c>
       <c r="B77" s="2">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>11</v>
@@ -3584,7 +3595,7 @@
         <v>146</v>
       </c>
       <c r="B78" s="2">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>11</v>
@@ -3601,7 +3612,7 @@
         <v>111</v>
       </c>
       <c r="B79" s="2">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>11</v>
@@ -3618,7 +3629,7 @@
         <v>147</v>
       </c>
       <c r="B80" s="2">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>11</v>
@@ -3635,7 +3646,7 @@
         <v>148</v>
       </c>
       <c r="B81" s="2">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>11</v>
@@ -3652,7 +3663,7 @@
         <v>112</v>
       </c>
       <c r="B82" s="2">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>11</v>
@@ -3669,7 +3680,7 @@
         <v>21</v>
       </c>
       <c r="B83" s="2">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>11</v>
@@ -3686,7 +3697,7 @@
         <v>22</v>
       </c>
       <c r="B84" s="2">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>11</v>
@@ -3703,7 +3714,7 @@
         <v>23</v>
       </c>
       <c r="B85" s="2">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>11</v>
@@ -3720,7 +3731,7 @@
         <v>24</v>
       </c>
       <c r="B86" s="2">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>11</v>
@@ -3737,7 +3748,7 @@
         <v>25</v>
       </c>
       <c r="B87" s="2">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>11</v>
@@ -3754,7 +3765,7 @@
         <v>26</v>
       </c>
       <c r="B88" s="2">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>11</v>
@@ -3771,7 +3782,7 @@
         <v>30</v>
       </c>
       <c r="B89" s="2">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>11</v>
@@ -3788,7 +3799,7 @@
         <v>31</v>
       </c>
       <c r="B90" s="2">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>11</v>
@@ -3805,7 +3816,7 @@
         <v>32</v>
       </c>
       <c r="B91" s="2">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>11</v>
@@ -3822,7 +3833,7 @@
         <v>33</v>
       </c>
       <c r="B92" s="2">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>11</v>
@@ -3839,7 +3850,7 @@
         <v>34</v>
       </c>
       <c r="B93" s="2">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>11</v>
@@ -3856,7 +3867,7 @@
         <v>40</v>
       </c>
       <c r="B94" s="2">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>11</v>
@@ -3873,7 +3884,7 @@
         <v>36</v>
       </c>
       <c r="B95" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>11</v>
@@ -3890,7 +3901,7 @@
         <v>37</v>
       </c>
       <c r="B96" s="2">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>11</v>
@@ -3907,7 +3918,7 @@
         <v>38</v>
       </c>
       <c r="B97" s="2">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>11</v>
@@ -3924,7 +3935,7 @@
         <v>39</v>
       </c>
       <c r="B98" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>11</v>
@@ -3941,7 +3952,7 @@
         <v>41</v>
       </c>
       <c r="B99" s="2">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>11</v>
@@ -3958,7 +3969,7 @@
         <v>42</v>
       </c>
       <c r="B100" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>11</v>
@@ -3975,7 +3986,7 @@
         <v>45</v>
       </c>
       <c r="B101" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>11</v>
@@ -3992,7 +4003,7 @@
         <v>46</v>
       </c>
       <c r="B102" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>11</v>
@@ -4009,7 +4020,7 @@
         <v>47</v>
       </c>
       <c r="B103" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>11</v>
@@ -4026,7 +4037,7 @@
         <v>48</v>
       </c>
       <c r="B104" s="2">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>11</v>
@@ -4043,7 +4054,7 @@
         <v>49</v>
       </c>
       <c r="B105" s="2">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>11</v>
@@ -4060,7 +4071,7 @@
         <v>53</v>
       </c>
       <c r="B106" s="2">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>11</v>
@@ -4077,7 +4088,7 @@
         <v>54</v>
       </c>
       <c r="B107" s="2">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>11</v>
@@ -4094,7 +4105,7 @@
         <v>55</v>
       </c>
       <c r="B108" s="2">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>11</v>
@@ -4111,7 +4122,7 @@
         <v>57</v>
       </c>
       <c r="B109" s="2">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>11</v>
@@ -4128,7 +4139,7 @@
         <v>149</v>
       </c>
       <c r="B110" s="2">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>11</v>
@@ -4145,7 +4156,7 @@
         <v>150</v>
       </c>
       <c r="B111" s="2">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>11</v>
@@ -4162,7 +4173,7 @@
         <v>63</v>
       </c>
       <c r="B112" s="2">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>11</v>
@@ -4179,7 +4190,7 @@
         <v>64</v>
       </c>
       <c r="B113" s="2">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>11</v>
@@ -4589,11 +4600,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="C1"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C113">
+    <dataValidation showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C113" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E113">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E113" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"High,Low"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4603,7 +4614,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>